<commit_message>
Summary parser updated, bug fixes on parser
</commit_message>
<xml_diff>
--- a/Datalogger Test Plan.xlsx
+++ b/Datalogger Test Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Test Name</t>
   </si>
@@ -27,24 +27,12 @@
     <t>Expected Results</t>
   </si>
   <si>
-    <t>Remove and reinsert SD card</t>
-  </si>
-  <si>
-    <t>Logger continues logging, no data is lost (minus during the time the SD card was missing).</t>
-  </si>
-  <si>
     <t>Repeat x Times</t>
   </si>
   <si>
-    <t>Remove SD card - record files. Wait a period of time (increase time for each test you do, between a few seconds to 15 minutes). Reinsert SD card. Wait 15 seconds. Remove SD card. See if datalogger contains same data + new data from those 15 seconds.</t>
-  </si>
-  <si>
     <t>Possible Failures</t>
   </si>
   <si>
-    <t xml:space="preserve">File is corrupted. New data is not recorded. </t>
-  </si>
-  <si>
     <t>Device continues to operate over long period of time, with no unexpected data loss. Data lost due to full SD card is expected, only the oldest data should be lost.</t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t>Logs from test.</t>
   </si>
   <si>
-    <t>Logs prior to and after each SD card removal.</t>
-  </si>
-  <si>
     <t>Checkmark.</t>
   </si>
   <si>
@@ -172,13 +157,25 @@
   </si>
   <si>
     <t>Same as above, but to 30C</t>
+  </si>
+  <si>
+    <t>Reboot</t>
+  </si>
+  <si>
+    <t>Device reboots. Continues to parse data. Only data lost is the data during the time that the device was rebootings.</t>
+  </si>
+  <si>
+    <t>Run logging. Force reboot device.</t>
+  </si>
+  <si>
+    <t>Datalogger does not resume logging immediately after reboot (waits until next cycle). Datalogger does not resume logging.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -224,6 +221,13 @@
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Times New Roman"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -285,7 +289,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -297,6 +301,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,11 +615,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -637,242 +644,242 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="95.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="3">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -913,14 +920,11 @@
     <row r="28" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-    </row>
+    <row r="29" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>